<commit_message>
added popup for WWTurl
</commit_message>
<xml_diff>
--- a/data/TileWallData/TileWallTables.xlsx
+++ b/data/TileWallData/TileWallTables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="720" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3800" yWindow="1540" windowWidth="28160" windowHeight="16880" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Galaxies" sheetId="1" r:id="rId1"/>
@@ -868,9 +868,6 @@
     <t>http://tilewall.adlerplanetarium.org:5050/layerApi.aspx?cmd=mode&amp;lookat=Sky&amp;flyto=31.1408333333333,20.8513888888889,10.8401140468817,-0.358141562509237,0</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>Alpha Centauri</t>
   </si>
   <si>
@@ -2412,6 +2409,9 @@
       </rPr>
       <t>, a face-on spiral galaxy distanced 21 million light-years (six megaparsecs) away.</t>
     </r>
+  </si>
+  <si>
+    <t>WWTurl</t>
   </si>
 </sst>
 </file>
@@ -2879,8 +2879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="A13:XFD13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2893,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>422</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -3453,7 +3453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -3464,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>422</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -3618,7 +3618,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3628,7 +3628,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>422</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -3933,7 +3933,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3943,7 +3943,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>422</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -3957,162 +3957,162 @@
     </row>
     <row r="2" spans="1:5" ht="300" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="209" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>234</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="287" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>237</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="225" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="235" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>247</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="209" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>250</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="222" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>254</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="248" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="225" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>260</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>261</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -4148,7 +4148,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4158,7 +4158,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>422</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -4172,155 +4172,155 @@
     </row>
     <row r="2" spans="1:5" ht="193" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="177" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="177" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>280</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>281</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>210</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="161" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>285</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="193" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>289</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="177" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>293</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="177" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="183" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>301</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="196" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="196" thickBot="1" x14ac:dyDescent="0.25">
@@ -4328,42 +4328,42 @@
         <v>57</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="225" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>307</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>308</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="287" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>310</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>311</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -4402,7 +4402,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B2" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4412,7 +4412,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>422</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -4426,315 +4426,315 @@
     </row>
     <row r="2" spans="1:5" ht="321" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="287" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>328</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>329</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="222" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>331</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>332</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="193" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>334</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>335</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="326" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>337</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>338</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="209" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>340</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>341</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="170" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>343</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>344</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="367" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>346</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>347</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5" ht="235" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>350</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>351</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>353</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>354</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>356</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>357</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="326" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>359</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>360</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="183" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="378" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>366</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>367</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="225" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>369</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>370</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="339" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>374</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="287" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>376</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>377</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="248" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>379</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>380</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>382</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>383</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>385</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>386</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -4812,8 +4812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4823,7 +4823,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>422</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -4837,291 +4837,291 @@
     </row>
     <row r="2" spans="1:5" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>328</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>329</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>376</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>377</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>340</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>341</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>331</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>332</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>350</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>396</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>351</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>385</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>386</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>353</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>354</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="338" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>416</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>369</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>370</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>334</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>335</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>325</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>326</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>366</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>367</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>359</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>399</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>360</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>337</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>338</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="169" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>343</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>344</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>356</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>357</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>364</v>
-      </c>
       <c r="E18" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>379</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>380</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="409" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>382</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>383</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>